<commit_message>
Updated the test file for example SIP book
</commit_message>
<xml_diff>
--- a/Future Value Article/test_1.xlsx
+++ b/Future Value Article/test_1.xlsx
@@ -1,27 +1,86 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimelbcloud-my.sharepoint.com/personal/stavyad_student_unimelb_edu_au/Documents/Medium Articles/Future Value Article/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="57" documentId="11_F25DC773A252ABDACC10484DE19E4ED85BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BD7172A-9927-4B61-BA1A-F4EB1E5F780D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Fund Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIP </t>
+  </si>
+  <si>
+    <t>Time (in months)</t>
+  </si>
+  <si>
+    <t>Final Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X Fund </t>
+  </si>
+  <si>
+    <t>Principle Investment</t>
+  </si>
+  <si>
+    <t>Y_Fund</t>
+  </si>
+  <si>
+    <t>Z_fund</t>
+  </si>
+  <si>
+    <t>Rate of Return (per month)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;₹&quot;\ #,##0.00;[Red]&quot;₹&quot;\ \-#,##0.00"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -49,8 +108,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +392,107 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>-1</v>
+      </c>
+      <c r="E2">
+        <v>-100</v>
+      </c>
+      <c r="F2" s="3">
+        <f>FV(B2,C2,D2,E2)</f>
+        <v>125.36500602639396</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="C3">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>-3</v>
+      </c>
+      <c r="E3">
+        <v>-50</v>
+      </c>
+      <c r="F3" s="3">
+        <f>FV(B3,C3,D3,E3)</f>
+        <v>171.68744989504501</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>-1100</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <f>FV(B4,C4,D4,E4)</f>
+        <v>7482.1040937499993</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>